<commit_message>
Report changes. Now for into conclusion etc.
</commit_message>
<xml_diff>
--- a/Open day poster/Project Data II.xlsx
+++ b/Open day poster/Project Data II.xlsx
@@ -460,16 +460,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +474,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -493,7 +493,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -595,7 +595,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -603,7 +603,7 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -765,12 +765,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="box"/>
-        <c:axId val="95766400"/>
-        <c:axId val="95767936"/>
+        <c:axId val="49566464"/>
+        <c:axId val="49568000"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="95766400"/>
+        <c:axId val="49566464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -787,14 +787,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95767936"/>
+        <c:crossAx val="49568000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95767936"/>
+        <c:axId val="49568000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95766400"/>
+        <c:crossAx val="49566464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,7 +836,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -844,7 +844,7 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1023,12 +1023,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="98641024"/>
-        <c:axId val="98642944"/>
+        <c:axId val="49631232"/>
+        <c:axId val="49633152"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98641024"/>
+        <c:axId val="49631232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,14 +1064,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98642944"/>
+        <c:crossAx val="49633152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98642944"/>
+        <c:axId val="49633152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,7 +1107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98641024"/>
+        <c:crossAx val="49631232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1130,7 +1130,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1138,7 +1138,7 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1319,12 +1319,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="box"/>
-        <c:axId val="98669696"/>
-        <c:axId val="98671232"/>
+        <c:axId val="49664000"/>
+        <c:axId val="49665536"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98669696"/>
+        <c:axId val="49664000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,14 +1341,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98671232"/>
+        <c:crossAx val="49665536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98671232"/>
+        <c:axId val="49665536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98669696"/>
+        <c:crossAx val="49664000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1390,7 +1390,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1398,7 +1398,7 @@
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1585,12 +1585,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="98976128"/>
-        <c:axId val="98978048"/>
+        <c:axId val="49757184"/>
+        <c:axId val="49796224"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98976128"/>
+        <c:axId val="49757184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,14 +1626,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98978048"/>
+        <c:crossAx val="49796224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98978048"/>
+        <c:axId val="49796224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98976128"/>
+        <c:crossAx val="49757184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1692,7 +1692,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1700,7 +1700,7 @@
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1784,12 +1784,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="98999680"/>
-        <c:axId val="99022336"/>
+        <c:axId val="49690880"/>
+        <c:axId val="49701248"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98999680"/>
+        <c:axId val="49690880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,14 +1825,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99022336"/>
+        <c:crossAx val="49701248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99022336"/>
+        <c:axId val="49701248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1868,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98999680"/>
+        <c:crossAx val="49690880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1891,7 +1891,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1899,7 +1899,7 @@
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2028,12 +2028,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="box"/>
-        <c:axId val="95840896"/>
-        <c:axId val="95846784"/>
+        <c:axId val="49735168"/>
+        <c:axId val="49736704"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="95840896"/>
+        <c:axId val="49735168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,14 +2051,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95846784"/>
+        <c:crossAx val="49736704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95846784"/>
+        <c:axId val="49736704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2077,7 +2077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95840896"/>
+        <c:crossAx val="49735168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2100,7 +2100,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2108,7 +2108,7 @@
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2227,7 +2227,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2235,7 +2235,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -2339,7 +2339,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2347,7 +2347,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -2480,7 +2480,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2488,7 +2488,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -2597,7 +2597,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2605,7 +2605,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -2714,7 +2714,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2722,7 +2722,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:style val="10"/>
   <c:chart>
     <c:title>
@@ -2759,7 +2759,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12243044619422568"/>
-          <c:y val="2.7777777777777811E-2"/>
+          <c:y val="2.7777777777777821E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -2846,7 +2846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2854,7 +2854,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2933,12 +2933,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="86864640"/>
-        <c:axId val="86866560"/>
+        <c:axId val="47353216"/>
+        <c:axId val="47367680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="86864640"/>
+        <c:axId val="47353216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2973,14 +2973,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86866560"/>
+        <c:crossAx val="47367680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86866560"/>
+        <c:axId val="47367680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3016,7 +3016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86864640"/>
+        <c:crossAx val="47353216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3026,7 +3026,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3034,7 +3034,7 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3118,12 +3118,12 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="88362368"/>
-        <c:axId val="88385024"/>
+        <c:axId val="49502464"/>
+        <c:axId val="49504640"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88362368"/>
+        <c:axId val="49502464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3158,14 +3158,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88385024"/>
+        <c:crossAx val="49504640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88385024"/>
+        <c:axId val="49504640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3201,7 +3201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88362368"/>
+        <c:crossAx val="49502464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3224,7 +3224,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3232,7 +3232,7 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-ZA"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3368,12 +3368,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="box"/>
-        <c:axId val="88369792"/>
-        <c:axId val="88404352"/>
+        <c:axId val="49542656"/>
+        <c:axId val="49544192"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88369792"/>
+        <c:axId val="49542656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3390,14 +3390,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88404352"/>
+        <c:crossAx val="49544192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88404352"/>
+        <c:axId val="49544192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3416,7 +3416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88369792"/>
+        <c:crossAx val="49542656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3439,7 +3439,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3691,14 +3691,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4273,8 +4273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J274"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179:H194"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4331,26 +4331,26 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="15.75">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="40"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="25"/>
       <c r="F7" s="10" t="s">
         <v>6</v>
@@ -4363,12 +4363,12 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13">
         <v>2</v>
@@ -4381,12 +4381,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16">
         <v>0</v>
@@ -4661,30 +4661,30 @@
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:10" ht="15.75">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="43" t="s">
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="45"/>
-      <c r="H51" s="43" t="s">
+      <c r="G51" s="42"/>
+      <c r="H51" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="I51" s="44"/>
-      <c r="J51" s="45"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="42"/>
     </row>
     <row r="52" spans="1:10" ht="45">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="46"/>
+      <c r="A52" s="43"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="43"/>
       <c r="G52" s="48"/>
       <c r="H52" s="10" t="s">
         <v>6</v>
@@ -4697,13 +4697,13 @@
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
       <c r="F53" s="12">
         <v>2</v>
       </c>
@@ -4719,13 +4719,13 @@
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="15">
         <v>2</v>
       </c>
@@ -4756,13 +4756,13 @@
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
       <c r="F56" s="12">
         <v>1</v>
       </c>
@@ -4778,13 +4778,13 @@
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
       <c r="F57" s="12">
         <v>2</v>
       </c>
@@ -4800,13 +4800,13 @@
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
       <c r="F58" s="12">
         <v>0</v>
       </c>
@@ -4992,13 +4992,13 @@
       </c>
     </row>
     <row r="95" spans="1:9" ht="45">
-      <c r="A95" s="46" t="s">
+      <c r="A95" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B95" s="47"/>
-      <c r="C95" s="47"/>
-      <c r="D95" s="47"/>
-      <c r="E95" s="47"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
       <c r="F95" s="10" t="s">
         <v>6</v>
       </c>
@@ -5010,13 +5010,13 @@
       </c>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="39" t="s">
+      <c r="A96" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="40"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
       <c r="F96" s="13">
         <v>2</v>
       </c>
@@ -5028,13 +5028,13 @@
       </c>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="37" t="s">
+      <c r="A97" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47"/>
       <c r="F97" s="16">
         <v>1</v>
       </c>
@@ -5055,12 +5055,12 @@
       </c>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="39" t="s">
+      <c r="A99" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="40"/>
-      <c r="C99" s="40"/>
-      <c r="D99" s="40"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
       <c r="E99" s="12"/>
       <c r="F99" s="13">
         <v>3</v>
@@ -5073,12 +5073,12 @@
       </c>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="37" t="s">
+      <c r="A100" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="38"/>
+      <c r="B100" s="47"/>
+      <c r="C100" s="47"/>
+      <c r="D100" s="47"/>
       <c r="E100" s="15"/>
       <c r="F100" s="16">
         <v>0</v>
@@ -5101,13 +5101,13 @@
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="39" t="s">
+      <c r="A102" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B102" s="40"/>
-      <c r="C102" s="40"/>
-      <c r="D102" s="40"/>
-      <c r="E102" s="40"/>
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
       <c r="F102" s="13">
         <v>10</v>
       </c>
@@ -5119,13 +5119,13 @@
       </c>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="37" t="s">
+      <c r="A103" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="38"/>
+      <c r="B103" s="47"/>
+      <c r="C103" s="47"/>
+      <c r="D103" s="47"/>
+      <c r="E103" s="47"/>
       <c r="F103" s="16">
         <v>14</v>
       </c>
@@ -5692,6 +5692,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A96:E96"/>
+    <mergeCell ref="A97:E97"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A102:E102"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:D7"/>
@@ -5708,12 +5714,6 @@
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A57:E57"/>
     <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A96:E96"/>
-    <mergeCell ref="A97:E97"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A102:E102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>